<commit_message>
Added color by sample type.
</commit_message>
<xml_diff>
--- a/Metadata-Table-Caucasus.xlsx
+++ b/Metadata-Table-Caucasus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyvas\Box\Leslie-CaucasusThesis\DZ_Data\Compiled_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA68F6-D1B9-4E0C-82FA-AFAE19EE6138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50714221-059D-497E-880A-E933CBCAA491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Longitude (°E)</t>
   </si>
   <si>
-    <t xml:space="preserve">Type           </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lithology    </t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>Reported Age</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1273,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1304,24 +1304,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="10">
         <v>43.094054999999997</v>
@@ -1330,24 +1330,24 @@
         <v>42.185533</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="4">
         <v>41.206848000000001</v>
@@ -1356,24 +1356,24 @@
         <v>48.265042000000001</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="4">
         <v>42.862588000000002</v>
@@ -1382,24 +1382,24 @@
         <v>42.032890999999999</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="4">
         <v>40.837370999999997</v>
@@ -1408,24 +1408,24 @@
         <v>48.334865999999998</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="4">
         <v>42.930970000000002</v>
@@ -1434,20 +1434,20 @@
         <v>42.11927</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="4">
         <v>40.984380000000002</v>
@@ -1456,20 +1456,20 @@
         <v>45.644599999999997</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D8" s="4">
         <v>42.018219999999999</v>
@@ -1478,20 +1478,20 @@
         <v>43.769820000000003</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>32</v>
       </c>
       <c r="D9" s="15">
         <v>41.41</v>
@@ -1500,17 +1500,17 @@
         <v>46.930999999999997</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="69" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="69" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" s="69">
@@ -1520,17 +1520,17 @@
         <v>42.309722222222199</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="71"/>
       <c r="H10" s="72"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="66">
@@ -1540,17 +1540,17 @@
         <v>45.6666666666666</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="67"/>
       <c r="H11" s="68"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="66">
@@ -1560,17 +1560,17 @@
         <v>45.313055555555501</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="67"/>
       <c r="H12" s="68"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="66">
@@ -1580,17 +1580,17 @@
         <v>42.635833333333302</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="67"/>
       <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="74"/>
       <c r="D14" s="73">
@@ -1600,17 +1600,17 @@
         <v>43.481111111111098</v>
       </c>
       <c r="F14" s="75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="76"/>
       <c r="H14" s="77"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>40</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="20">
@@ -1620,24 +1620,24 @@
         <v>41.055833333333297</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="22" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="D16" s="25">
         <v>43.091799999999999</v>
@@ -1646,24 +1646,24 @@
         <v>42.293129999999998</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="26">
         <v>43.075940000000003</v>
@@ -1672,24 +1672,24 @@
         <v>42.2883</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>49</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D18" s="26">
         <v>43.078980000000001</v>
@@ -1698,24 +1698,24 @@
         <v>42.296019999999999</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="D19" s="26">
         <v>43.161389999999997</v>
@@ -1724,24 +1724,24 @@
         <v>42.405099999999997</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>56</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D20" s="26">
         <v>43.011839999999999</v>
@@ -1750,24 +1750,24 @@
         <v>42.591560000000001</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D21" s="26">
         <v>42.709670000000003</v>
@@ -1776,24 +1776,24 @@
         <v>44.627800000000001</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="33" t="s">
         <v>63</v>
-      </c>
-      <c r="H21" s="33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D22" s="26">
         <v>42.706670000000003</v>
@@ -1802,24 +1802,24 @@
         <v>44.631149999999998</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="H22" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>70</v>
       </c>
       <c r="D23" s="27">
         <v>42.717210000000001</v>
@@ -1828,24 +1828,24 @@
         <v>44.627119999999998</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="C24" s="37" t="s">
         <v>73</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>74</v>
       </c>
       <c r="D24" s="48">
         <v>42.116599999999998</v>
@@ -1854,20 +1854,20 @@
         <v>43.198398599999997</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="39"/>
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="38" t="s">
         <v>75</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>76</v>
       </c>
       <c r="D25" s="44">
         <v>42.364799499999997</v>
@@ -1876,20 +1876,20 @@
         <v>44.722999600000001</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="40"/>
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="38" t="s">
         <v>77</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>78</v>
       </c>
       <c r="D26" s="44">
         <v>42.221900900000001</v>
@@ -1898,20 +1898,20 @@
         <v>44.838798500000003</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" s="40"/>
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>79</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>80</v>
       </c>
       <c r="D27" s="44">
         <v>41.771099100000001</v>
@@ -1920,20 +1920,20 @@
         <v>45.150699600000003</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" s="40"/>
       <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="38" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>82</v>
       </c>
       <c r="D28" s="44">
         <v>41.844299300000003</v>
@@ -1942,20 +1942,20 @@
         <v>45.133300800000001</v>
       </c>
       <c r="F28" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="40"/>
       <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="38" t="s">
         <v>83</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>84</v>
       </c>
       <c r="D29" s="44">
         <v>41.908000899999998</v>
@@ -1964,20 +1964,20 @@
         <v>43.4734993</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" s="40"/>
       <c r="H29" s="50"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="38" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>86</v>
       </c>
       <c r="D30" s="44">
         <v>41.880600000000001</v>
@@ -1986,20 +1986,20 @@
         <v>44.326698299999997</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G30" s="40"/>
       <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="38" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>88</v>
       </c>
       <c r="D31" s="44">
         <v>41.515098600000002</v>
@@ -2008,20 +2008,20 @@
         <v>44.768199899999999</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31" s="40"/>
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="38" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>90</v>
       </c>
       <c r="D32" s="44">
         <v>41.406501800000001</v>
@@ -2030,20 +2030,20 @@
         <v>44.824401899999998</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" s="40"/>
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>91</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>92</v>
       </c>
       <c r="D33" s="44">
         <v>43.143901800000002</v>
@@ -2052,20 +2052,20 @@
         <v>42.402000399999999</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G33" s="40"/>
       <c r="H33" s="50"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="38" t="s">
         <v>93</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>94</v>
       </c>
       <c r="D34" s="44">
         <v>42.983001700000003</v>
@@ -2074,20 +2074,20 @@
         <v>42.240200000000002</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" s="40"/>
       <c r="H34" s="50"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="38" t="s">
         <v>95</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>96</v>
       </c>
       <c r="D35" s="44">
         <v>42.654399900000001</v>
@@ -2096,20 +2096,20 @@
         <v>42.215099299999999</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G35" s="40"/>
       <c r="H35" s="50"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="38" t="s">
         <v>97</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>98</v>
       </c>
       <c r="D36" s="44">
         <v>42.632099199999999</v>
@@ -2118,20 +2118,20 @@
         <v>42.168998700000003</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" s="40"/>
       <c r="H36" s="50"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>99</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>100</v>
       </c>
       <c r="D37" s="44">
         <v>42.661998699999998</v>
@@ -2140,20 +2140,20 @@
         <v>42.133499100000002</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="40"/>
       <c r="H37" s="50"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="38" t="s">
         <v>101</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>102</v>
       </c>
       <c r="D38" s="44">
         <v>42.644401600000002</v>
@@ -2162,20 +2162,20 @@
         <v>42.087398499999999</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G38" s="40"/>
       <c r="H38" s="50"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="38" t="s">
         <v>103</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>104</v>
       </c>
       <c r="D39" s="44">
         <v>42.6587982</v>
@@ -2184,20 +2184,20 @@
         <v>42.078601800000001</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G39" s="40"/>
       <c r="H39" s="50"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="38" t="s">
         <v>105</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>106</v>
       </c>
       <c r="D40" s="44">
         <v>42.4314003</v>
@@ -2206,20 +2206,20 @@
         <v>41.811599700000002</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" s="40"/>
       <c r="H40" s="50"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="38" t="s">
         <v>107</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>108</v>
       </c>
       <c r="D41" s="44">
         <v>41.145104600000003</v>
@@ -2228,20 +2228,20 @@
         <v>48.0635069</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G41" s="40"/>
       <c r="H41" s="50"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="38" t="s">
         <v>109</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>110</v>
       </c>
       <c r="D42" s="44">
         <v>40.942757899999997</v>
@@ -2250,20 +2250,20 @@
         <v>48.361635700000001</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G42" s="40"/>
       <c r="H42" s="50"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="38" t="s">
         <v>111</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>112</v>
       </c>
       <c r="D43" s="44">
         <v>41.036014999999999</v>
@@ -2272,20 +2272,20 @@
         <v>49.121131699999999</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G43" s="40"/>
       <c r="H43" s="50"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="38" t="s">
         <v>113</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>114</v>
       </c>
       <c r="D44" s="44">
         <v>40.8804546</v>
@@ -2294,20 +2294,20 @@
         <v>48.424571399999998</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44" s="40"/>
       <c r="H44" s="50"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="38" t="s">
         <v>115</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>116</v>
       </c>
       <c r="D45" s="44">
         <v>40.8180008</v>
@@ -2316,20 +2316,20 @@
         <v>48.318298300000002</v>
       </c>
       <c r="F45" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G45" s="40"/>
       <c r="H45" s="50"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="38" t="s">
         <v>117</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>118</v>
       </c>
       <c r="D46" s="44">
         <v>40.8364963</v>
@@ -2338,20 +2338,20 @@
         <v>48.387708400000001</v>
       </c>
       <c r="F46" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G46" s="40"/>
       <c r="H46" s="50"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>120</v>
       </c>
       <c r="D47" s="44">
         <v>40.725801699999998</v>
@@ -2360,20 +2360,20 @@
         <v>48.297331700000001</v>
       </c>
       <c r="F47" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G47" s="40"/>
       <c r="H47" s="50"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="38" t="s">
         <v>121</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>122</v>
       </c>
       <c r="D48" s="44">
         <v>41.180151700000003</v>
@@ -2382,20 +2382,20 @@
         <v>48.615465</v>
       </c>
       <c r="F48" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G48" s="40"/>
       <c r="H48" s="50"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="38" t="s">
         <v>123</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>124</v>
       </c>
       <c r="D49" s="44">
         <v>40.768374999999999</v>
@@ -2404,20 +2404,20 @@
         <v>48.301026700000001</v>
       </c>
       <c r="F49" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G49" s="40"/>
       <c r="H49" s="50"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="38" t="s">
         <v>125</v>
-      </c>
-      <c r="C50" s="38" t="s">
-        <v>126</v>
       </c>
       <c r="D50" s="44">
         <v>40.846670000000003</v>
@@ -2426,20 +2426,20 @@
         <v>48.380823300000003</v>
       </c>
       <c r="F50" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G50" s="40"/>
       <c r="H50" s="50"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="38" t="s">
         <v>127</v>
-      </c>
-      <c r="C51" s="38" t="s">
-        <v>128</v>
       </c>
       <c r="D51" s="44">
         <v>40.630119999999998</v>
@@ -2448,20 +2448,20 @@
         <v>48.473120700000003</v>
       </c>
       <c r="F51" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G51" s="40"/>
       <c r="H51" s="50"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>129</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>130</v>
       </c>
       <c r="D52" s="44">
         <v>40.5847233</v>
@@ -2470,20 +2470,20 @@
         <v>48.773310000000002</v>
       </c>
       <c r="F52" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G52" s="40"/>
       <c r="H52" s="50"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="41" t="s">
         <v>131</v>
-      </c>
-      <c r="C53" s="41" t="s">
-        <v>132</v>
       </c>
       <c r="D53" s="51">
         <v>40.465801200000001</v>
@@ -2492,20 +2492,20 @@
         <v>48.686401400000001</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G53" s="42"/>
       <c r="H53" s="52"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="C54" s="46" t="s">
         <v>134</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>135</v>
       </c>
       <c r="D54" s="53">
         <v>43.0045</v>
@@ -2514,20 +2514,20 @@
         <v>42.299399999999999</v>
       </c>
       <c r="F54" s="56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G54" s="57"/>
       <c r="H54" s="58"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="45" t="s">
         <v>136</v>
-      </c>
-      <c r="C55" s="45" t="s">
-        <v>137</v>
       </c>
       <c r="D55" s="54">
         <v>42.734699999999997</v>
@@ -2536,20 +2536,20 @@
         <v>42.762900000000002</v>
       </c>
       <c r="F55" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G55" s="64"/>
       <c r="H55" s="59"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="45" t="s">
         <v>138</v>
-      </c>
-      <c r="C56" s="45" t="s">
-        <v>139</v>
       </c>
       <c r="D56" s="54">
         <v>42.410899999999998</v>
@@ -2558,20 +2558,20 @@
         <v>44.607500000000002</v>
       </c>
       <c r="F56" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G56" s="64"/>
       <c r="H56" s="59"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B57" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="45" t="s">
         <v>140</v>
-      </c>
-      <c r="C57" s="45" t="s">
-        <v>141</v>
       </c>
       <c r="D57" s="54">
         <v>42.180999999999997</v>
@@ -2580,20 +2580,20 @@
         <v>45.435600000000001</v>
       </c>
       <c r="F57" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G57" s="64"/>
       <c r="H57" s="60"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="45" t="s">
         <v>142</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>143</v>
       </c>
       <c r="D58" s="54">
         <v>41.706699999999998</v>
@@ -2602,20 +2602,20 @@
         <v>46.5931</v>
       </c>
       <c r="F58" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G58" s="64"/>
       <c r="H58" s="59"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="45" t="s">
         <v>144</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>145</v>
       </c>
       <c r="D59" s="54">
         <v>41.256599999999999</v>
@@ -2624,20 +2624,20 @@
         <v>47.221299999999999</v>
       </c>
       <c r="F59" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G59" s="40"/>
       <c r="H59" s="59"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="47" t="s">
         <v>146</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>147</v>
       </c>
       <c r="D60" s="55">
         <v>41.0672</v>
@@ -2646,7 +2646,7 @@
         <v>47.792400000000001</v>
       </c>
       <c r="F60" s="65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G60" s="61"/>
       <c r="H60" s="62"/>

</xml_diff>

<commit_message>
Minor corrections and added catchment data.
</commit_message>
<xml_diff>
--- a/Metadata-Table-Caucasus.xlsx
+++ b/Metadata-Table-Caucasus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyvas\Box\Leslie-CaucasusThesis\DZ_Data\Compiled_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50714221-059D-497E-880A-E933CBCAA491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8536C7-D835-45E5-A65F-E3C46A868DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2512" yWindow="2512" windowWidth="16876" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="158">
   <si>
     <t>Source</t>
   </si>
@@ -135,9 +135,6 @@
     <t>WG951</t>
   </si>
   <si>
-    <t>ILN-13_700-706</t>
-  </si>
-  <si>
     <t>WC1391</t>
   </si>
   <si>
@@ -481,13 +478,40 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Sublitharenite</t>
+  </si>
+  <si>
+    <t>Oligocene</t>
+  </si>
+  <si>
+    <t>Chattian–Aquitanian</t>
+  </si>
+  <si>
+    <t>ILN-13_700</t>
+  </si>
+  <si>
+    <t>Late Messinian–Zanclean</t>
+  </si>
+  <si>
+    <t>Quartz arenite</t>
+  </si>
+  <si>
+    <t>Lithic arenite</t>
+  </si>
+  <si>
+    <t>Langhian</t>
+  </si>
+  <si>
+    <t>Mid Rupelian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,11 +531,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -542,6 +561,18 @@
       <color rgb="FF000000"/>
       <name val="Times Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -557,7 +588,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -753,26 +784,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFA6A6A6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -781,14 +801,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -813,30 +830,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,9 +862,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -863,20 +874,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -886,13 +897,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,39 +933,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,8 +1281,8 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1292,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1304,43 +1313,43 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>43.094054999999997</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>42.185533</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1361,12 +1370,12 @@
       <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1387,12 +1396,12 @@
       <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1413,12 +1422,12 @@
       <c r="G5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1437,10 +1446,10 @@
         <v>25</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1459,10 +1468,10 @@
         <v>25</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1481,1179 +1490,1191 @@
         <v>25</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>41.41</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>46.930999999999997</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17"/>
+      <c r="F9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="69">
+      <c r="D10" s="65">
+        <v>42.309722222222199</v>
+      </c>
+      <c r="E10" s="65">
         <v>43.485833333333296</v>
       </c>
-      <c r="E10" s="69">
-        <v>42.309722222222199</v>
-      </c>
-      <c r="F10" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="71"/>
-      <c r="H10" s="72"/>
+      <c r="F10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="63">
+        <v>45.6666666666666</v>
+      </c>
+      <c r="E11" s="63">
+        <v>40.8333333333333</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="66">
-        <v>40.8333333333333</v>
-      </c>
-      <c r="E11" s="66">
-        <v>45.6666666666666</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="9" t="s">
+      <c r="D12" s="63">
+        <v>45.313055555555501</v>
+      </c>
+      <c r="E12" s="63">
+        <v>37.010833333333302</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B13" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="66">
-        <v>37.010833333333302</v>
-      </c>
-      <c r="E12" s="66">
-        <v>45.313055555555501</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="9" t="s">
+      <c r="D13" s="63">
+        <v>42.635833333333302</v>
+      </c>
+      <c r="E13" s="63">
+        <v>42.7361111111111</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B14" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="66">
-        <v>42.7361111111111</v>
-      </c>
-      <c r="E13" s="66">
-        <v>42.635833333333302</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="73" t="s">
+      <c r="D14" s="66">
+        <v>43.481111111111098</v>
+      </c>
+      <c r="E14" s="66">
+        <v>40.0411111111111</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="67"/>
+      <c r="H14" s="73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="73">
-        <v>40.0411111111111</v>
-      </c>
-      <c r="E14" s="73">
-        <v>43.481111111111098</v>
-      </c>
-      <c r="F14" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="76"/>
-      <c r="H14" s="77"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="D15" s="18">
+        <v>41.055833333333297</v>
+      </c>
+      <c r="E15" s="18">
+        <v>48.5891666666666</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="20">
-        <v>48.5891666666666</v>
-      </c>
-      <c r="E15" s="20">
-        <v>41.055833333333297</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="20" t="s">
+      <c r="H15" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="D16" s="23">
+        <v>43.091799999999999</v>
+      </c>
+      <c r="E16" s="23">
+        <v>42.293129999999998</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="25">
-        <v>43.091799999999999</v>
-      </c>
-      <c r="E16" s="25">
-        <v>42.293129999999998</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="25" t="s">
+      <c r="H16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="34" t="s">
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="24">
+        <v>43.075940000000003</v>
+      </c>
+      <c r="E17" s="24">
+        <v>42.2883</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="26">
-        <v>43.075940000000003</v>
-      </c>
-      <c r="E17" s="26">
-        <v>42.2883</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="26" t="s">
+      <c r="H17" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="32" t="s">
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="24">
+        <v>43.078980000000001</v>
+      </c>
+      <c r="E18" s="24">
+        <v>42.296019999999999</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="26">
-        <v>43.078980000000001</v>
-      </c>
-      <c r="E18" s="26">
-        <v>42.296019999999999</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="32" t="s">
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="24">
+        <v>43.161389999999997</v>
+      </c>
+      <c r="E19" s="24">
+        <v>42.405099999999997</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="26">
-        <v>43.161389999999997</v>
-      </c>
-      <c r="E19" s="26">
-        <v>42.405099999999997</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="26" t="s">
+      <c r="H19" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="32" t="s">
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="24">
+        <v>43.011839999999999</v>
+      </c>
+      <c r="E20" s="24">
+        <v>42.591560000000001</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="26">
-        <v>43.011839999999999</v>
-      </c>
-      <c r="E20" s="26">
-        <v>42.591560000000001</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="32" t="s">
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="24">
+        <v>42.709670000000003</v>
+      </c>
+      <c r="E21" s="24">
+        <v>44.627800000000001</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="26">
-        <v>42.709670000000003</v>
-      </c>
-      <c r="E21" s="26">
-        <v>44.627800000000001</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="26" t="s">
+      <c r="H21" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="33" t="s">
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="24">
+        <v>42.706670000000003</v>
+      </c>
+      <c r="E22" s="24">
+        <v>44.631149999999998</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="26">
-        <v>42.706670000000003</v>
-      </c>
-      <c r="E22" s="26">
-        <v>44.631149999999998</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="26" t="s">
+      <c r="H22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="33" t="s">
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="23" t="s">
+      <c r="C23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="D23" s="25">
+        <v>42.717210000000001</v>
+      </c>
+      <c r="E23" s="25">
+        <v>44.627119999999998</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="27">
-        <v>42.717210000000001</v>
-      </c>
-      <c r="E23" s="27">
-        <v>44.627119999999998</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="C24" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="D24" s="45">
+        <v>42.116599999999998</v>
+      </c>
+      <c r="E24" s="45">
+        <v>43.198398599999997</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="46"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="48">
-        <v>42.116599999999998</v>
-      </c>
-      <c r="E24" s="48">
-        <v>43.198398599999997</v>
-      </c>
-      <c r="F24" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="49"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="38" t="s">
+      <c r="C25" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="D25" s="41">
+        <v>42.364799499999997</v>
+      </c>
+      <c r="E25" s="41">
+        <v>44.722999600000001</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="37"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="44">
-        <v>42.364799499999997</v>
-      </c>
-      <c r="E25" s="44">
-        <v>44.722999600000001</v>
-      </c>
-      <c r="F25" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="40"/>
-      <c r="H25" s="50"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="38" t="s">
+      <c r="C26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="D26" s="41">
+        <v>42.221900900000001</v>
+      </c>
+      <c r="E26" s="41">
+        <v>44.838798500000003</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="37"/>
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="44">
-        <v>42.221900900000001</v>
-      </c>
-      <c r="E26" s="44">
-        <v>44.838798500000003</v>
-      </c>
-      <c r="F26" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="50"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="38" t="s">
+      <c r="C27" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="D27" s="41">
+        <v>41.771099100000001</v>
+      </c>
+      <c r="E27" s="41">
+        <v>45.150699600000003</v>
+      </c>
+      <c r="F27" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="44">
-        <v>41.771099100000001</v>
-      </c>
-      <c r="E27" s="44">
-        <v>45.150699600000003</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="38" t="s">
+      <c r="C28" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="D28" s="41">
+        <v>41.844299300000003</v>
+      </c>
+      <c r="E28" s="41">
+        <v>45.133300800000001</v>
+      </c>
+      <c r="F28" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="44">
-        <v>41.844299300000003</v>
-      </c>
-      <c r="E28" s="44">
-        <v>45.133300800000001</v>
-      </c>
-      <c r="F28" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="50"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="38" t="s">
+      <c r="C29" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="D29" s="41">
+        <v>41.908000899999998</v>
+      </c>
+      <c r="E29" s="41">
+        <v>43.4734993</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="44">
-        <v>41.908000899999998</v>
-      </c>
-      <c r="E29" s="44">
-        <v>43.4734993</v>
-      </c>
-      <c r="F29" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="38" t="s">
+      <c r="C30" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="D30" s="41">
+        <v>41.880600000000001</v>
+      </c>
+      <c r="E30" s="41">
+        <v>44.326698299999997</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="47"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="44">
-        <v>41.880600000000001</v>
-      </c>
-      <c r="E30" s="44">
-        <v>44.326698299999997</v>
-      </c>
-      <c r="F30" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="50"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="38" t="s">
+      <c r="C31" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="D31" s="41">
+        <v>41.515098600000002</v>
+      </c>
+      <c r="E31" s="41">
+        <v>44.768199899999999</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="37"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="44">
-        <v>41.515098600000002</v>
-      </c>
-      <c r="E31" s="44">
-        <v>44.768199899999999</v>
-      </c>
-      <c r="F31" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="38" t="s">
+      <c r="C32" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="D32" s="41">
+        <v>41.406501800000001</v>
+      </c>
+      <c r="E32" s="41">
+        <v>44.824401899999998</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="37"/>
+      <c r="H32" s="47"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="44">
-        <v>41.406501800000001</v>
-      </c>
-      <c r="E32" s="44">
-        <v>44.824401899999998</v>
-      </c>
-      <c r="F32" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="40"/>
-      <c r="H32" s="50"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="38" t="s">
+      <c r="C33" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="D33" s="41">
+        <v>43.143901800000002</v>
+      </c>
+      <c r="E33" s="41">
+        <v>42.402000399999999</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="37"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="44">
-        <v>43.143901800000002</v>
-      </c>
-      <c r="E33" s="44">
-        <v>42.402000399999999</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="40"/>
-      <c r="H33" s="50"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="38" t="s">
+      <c r="C34" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="D34" s="41">
+        <v>42.983001700000003</v>
+      </c>
+      <c r="E34" s="41">
+        <v>42.240200000000002</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="37"/>
+      <c r="H34" s="47"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="44">
-        <v>42.983001700000003</v>
-      </c>
-      <c r="E34" s="44">
-        <v>42.240200000000002</v>
-      </c>
-      <c r="F34" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="40"/>
-      <c r="H34" s="50"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="38" t="s">
+      <c r="C35" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="D35" s="41">
+        <v>42.654399900000001</v>
+      </c>
+      <c r="E35" s="41">
+        <v>42.215099299999999</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="37"/>
+      <c r="H35" s="47"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="44">
-        <v>42.654399900000001</v>
-      </c>
-      <c r="E35" s="44">
-        <v>42.215099299999999</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="40"/>
-      <c r="H35" s="50"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="38" t="s">
+      <c r="C36" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="D36" s="41">
+        <v>42.632099199999999</v>
+      </c>
+      <c r="E36" s="41">
+        <v>42.168998700000003</v>
+      </c>
+      <c r="F36" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="37"/>
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="44">
-        <v>42.632099199999999</v>
-      </c>
-      <c r="E36" s="44">
-        <v>42.168998700000003</v>
-      </c>
-      <c r="F36" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="40"/>
-      <c r="H36" s="50"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="38" t="s">
+      <c r="C37" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="D37" s="41">
+        <v>42.661998699999998</v>
+      </c>
+      <c r="E37" s="41">
+        <v>42.133499100000002</v>
+      </c>
+      <c r="F37" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="37"/>
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="44">
-        <v>42.661998699999998</v>
-      </c>
-      <c r="E37" s="44">
-        <v>42.133499100000002</v>
-      </c>
-      <c r="F37" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="50"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="38" t="s">
+      <c r="C38" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="D38" s="41">
+        <v>42.644401600000002</v>
+      </c>
+      <c r="E38" s="41">
+        <v>42.087398499999999</v>
+      </c>
+      <c r="F38" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="37"/>
+      <c r="H38" s="47"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="44">
-        <v>42.644401600000002</v>
-      </c>
-      <c r="E38" s="44">
-        <v>42.087398499999999</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="40"/>
-      <c r="H38" s="50"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="38" t="s">
+      <c r="C39" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="D39" s="41">
+        <v>42.6587982</v>
+      </c>
+      <c r="E39" s="41">
+        <v>42.078601800000001</v>
+      </c>
+      <c r="F39" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="37"/>
+      <c r="H39" s="47"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="44">
-        <v>42.6587982</v>
-      </c>
-      <c r="E39" s="44">
-        <v>42.078601800000001</v>
-      </c>
-      <c r="F39" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="40"/>
-      <c r="H39" s="50"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="38" t="s">
+      <c r="C40" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="D40" s="41">
+        <v>42.4314003</v>
+      </c>
+      <c r="E40" s="41">
+        <v>41.811599700000002</v>
+      </c>
+      <c r="F40" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="37"/>
+      <c r="H40" s="47"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="44">
-        <v>42.4314003</v>
-      </c>
-      <c r="E40" s="44">
-        <v>41.811599700000002</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="40"/>
-      <c r="H40" s="50"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="38" t="s">
+      <c r="C41" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="D41" s="41">
+        <v>41.145104600000003</v>
+      </c>
+      <c r="E41" s="41">
+        <v>48.0635069</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="37"/>
+      <c r="H41" s="47"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="44">
-        <v>41.145104600000003</v>
-      </c>
-      <c r="E41" s="44">
-        <v>48.0635069</v>
-      </c>
-      <c r="F41" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="40"/>
-      <c r="H41" s="50"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="38" t="s">
+      <c r="C42" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="D42" s="41">
+        <v>40.942757899999997</v>
+      </c>
+      <c r="E42" s="41">
+        <v>48.361635700000001</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="37"/>
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="44">
-        <v>40.942757899999997</v>
-      </c>
-      <c r="E42" s="44">
-        <v>48.361635700000001</v>
-      </c>
-      <c r="F42" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="40"/>
-      <c r="H42" s="50"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="38" t="s">
+      <c r="C43" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="D43" s="41">
+        <v>41.036014999999999</v>
+      </c>
+      <c r="E43" s="41">
+        <v>49.121131699999999</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="37"/>
+      <c r="H43" s="47"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="44">
-        <v>41.036014999999999</v>
-      </c>
-      <c r="E43" s="44">
-        <v>49.121131699999999</v>
-      </c>
-      <c r="F43" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="40"/>
-      <c r="H43" s="50"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="38" t="s">
+      <c r="C44" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="D44" s="41">
+        <v>40.8804546</v>
+      </c>
+      <c r="E44" s="41">
+        <v>48.424571399999998</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="37"/>
+      <c r="H44" s="47"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="44">
-        <v>40.8804546</v>
-      </c>
-      <c r="E44" s="44">
-        <v>48.424571399999998</v>
-      </c>
-      <c r="F44" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="40"/>
-      <c r="H44" s="50"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="38" t="s">
+      <c r="C45" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="D45" s="41">
+        <v>40.8180008</v>
+      </c>
+      <c r="E45" s="41">
+        <v>48.318298300000002</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="37"/>
+      <c r="H45" s="47"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="44">
-        <v>40.8180008</v>
-      </c>
-      <c r="E45" s="44">
-        <v>48.318298300000002</v>
-      </c>
-      <c r="F45" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="40"/>
-      <c r="H45" s="50"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="38" t="s">
+      <c r="C46" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="D46" s="41">
+        <v>40.8364963</v>
+      </c>
+      <c r="E46" s="41">
+        <v>48.387708400000001</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="37"/>
+      <c r="H46" s="47"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="D46" s="44">
-        <v>40.8364963</v>
-      </c>
-      <c r="E46" s="44">
-        <v>48.387708400000001</v>
-      </c>
-      <c r="F46" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="40"/>
-      <c r="H46" s="50"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="38" t="s">
+      <c r="C47" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="D47" s="41">
+        <v>40.725801699999998</v>
+      </c>
+      <c r="E47" s="41">
+        <v>48.297331700000001</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="37"/>
+      <c r="H47" s="47"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="44">
-        <v>40.725801699999998</v>
-      </c>
-      <c r="E47" s="44">
-        <v>48.297331700000001</v>
-      </c>
-      <c r="F47" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="40"/>
-      <c r="H47" s="50"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="38" t="s">
+      <c r="C48" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="D48" s="41">
+        <v>41.180151700000003</v>
+      </c>
+      <c r="E48" s="41">
+        <v>48.615465</v>
+      </c>
+      <c r="F48" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="37"/>
+      <c r="H48" s="47"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="44">
-        <v>41.180151700000003</v>
-      </c>
-      <c r="E48" s="44">
-        <v>48.615465</v>
-      </c>
-      <c r="F48" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="40"/>
-      <c r="H48" s="50"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="38" t="s">
+      <c r="C49" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="D49" s="41">
+        <v>40.768374999999999</v>
+      </c>
+      <c r="E49" s="41">
+        <v>48.301026700000001</v>
+      </c>
+      <c r="F49" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="37"/>
+      <c r="H49" s="47"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="D49" s="44">
-        <v>40.768374999999999</v>
-      </c>
-      <c r="E49" s="44">
-        <v>48.301026700000001</v>
-      </c>
-      <c r="F49" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="40"/>
-      <c r="H49" s="50"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="38" t="s">
+      <c r="C50" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="D50" s="41">
+        <v>40.846670000000003</v>
+      </c>
+      <c r="E50" s="41">
+        <v>48.380823300000003</v>
+      </c>
+      <c r="F50" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="37"/>
+      <c r="H50" s="47"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="D50" s="44">
-        <v>40.846670000000003</v>
-      </c>
-      <c r="E50" s="44">
-        <v>48.380823300000003</v>
-      </c>
-      <c r="F50" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="40"/>
-      <c r="H50" s="50"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="38" t="s">
+      <c r="C51" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C51" s="38" t="s">
+      <c r="D51" s="41">
+        <v>40.630119999999998</v>
+      </c>
+      <c r="E51" s="41">
+        <v>48.473120700000003</v>
+      </c>
+      <c r="F51" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="37"/>
+      <c r="H51" s="47"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="44">
-        <v>40.630119999999998</v>
-      </c>
-      <c r="E51" s="44">
-        <v>48.473120700000003</v>
-      </c>
-      <c r="F51" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G51" s="40"/>
-      <c r="H51" s="50"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="38" t="s">
+      <c r="C52" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="D52" s="41">
+        <v>40.5847233</v>
+      </c>
+      <c r="E52" s="41">
+        <v>48.773310000000002</v>
+      </c>
+      <c r="F52" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="37"/>
+      <c r="H52" s="47"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="44">
-        <v>40.5847233</v>
-      </c>
-      <c r="E52" s="44">
-        <v>48.773310000000002</v>
-      </c>
-      <c r="F52" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="40"/>
-      <c r="H52" s="50"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B53" s="41" t="s">
+      <c r="C53" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="D53" s="48">
+        <v>40.465801200000001</v>
+      </c>
+      <c r="E53" s="48">
+        <v>48.686401400000001</v>
+      </c>
+      <c r="F53" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="39"/>
+      <c r="H53" s="49"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="51">
-        <v>40.465801200000001</v>
-      </c>
-      <c r="E53" s="51">
-        <v>48.686401400000001</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="42"/>
-      <c r="H53" s="52"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="43" t="s">
+      <c r="B54" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="C54" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="D54" s="50">
+        <v>43.0045</v>
+      </c>
+      <c r="E54" s="50">
+        <v>42.299399999999999</v>
+      </c>
+      <c r="F54" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="54"/>
+      <c r="H54" s="55"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="53">
-        <v>43.0045</v>
-      </c>
-      <c r="E54" s="53">
-        <v>42.299399999999999</v>
-      </c>
-      <c r="F54" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="57"/>
-      <c r="H54" s="58"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="45" t="s">
+      <c r="C55" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="D55" s="51">
+        <v>42.734699999999997</v>
+      </c>
+      <c r="E55" s="51">
+        <v>42.762900000000002</v>
+      </c>
+      <c r="F55" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="61"/>
+      <c r="H55" s="56"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="D55" s="54">
-        <v>42.734699999999997</v>
-      </c>
-      <c r="E55" s="54">
-        <v>42.762900000000002</v>
-      </c>
-      <c r="F55" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G55" s="64"/>
-      <c r="H55" s="59"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="45" t="s">
+      <c r="C56" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C56" s="45" t="s">
+      <c r="D56" s="51">
+        <v>42.410899999999998</v>
+      </c>
+      <c r="E56" s="51">
+        <v>44.607500000000002</v>
+      </c>
+      <c r="F56" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="61"/>
+      <c r="H56" s="56"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="54">
-        <v>42.410899999999998</v>
-      </c>
-      <c r="E56" s="54">
-        <v>44.607500000000002</v>
-      </c>
-      <c r="F56" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G56" s="64"/>
-      <c r="H56" s="59"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B57" s="45" t="s">
+      <c r="C57" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C57" s="45" t="s">
+      <c r="D57" s="51">
+        <v>42.180999999999997</v>
+      </c>
+      <c r="E57" s="51">
+        <v>45.435600000000001</v>
+      </c>
+      <c r="F57" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="61"/>
+      <c r="H57" s="57"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="D57" s="54">
-        <v>42.180999999999997</v>
-      </c>
-      <c r="E57" s="54">
-        <v>45.435600000000001</v>
-      </c>
-      <c r="F57" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="64"/>
-      <c r="H57" s="60"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="45" t="s">
+      <c r="C58" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="D58" s="51">
+        <v>41.706699999999998</v>
+      </c>
+      <c r="E58" s="51">
+        <v>46.5931</v>
+      </c>
+      <c r="F58" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="61"/>
+      <c r="H58" s="56"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="54">
-        <v>41.706699999999998</v>
-      </c>
-      <c r="E58" s="54">
-        <v>46.5931</v>
-      </c>
-      <c r="F58" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="64"/>
-      <c r="H58" s="59"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B59" s="45" t="s">
+      <c r="C59" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="D59" s="51">
+        <v>41.256599999999999</v>
+      </c>
+      <c r="E59" s="51">
+        <v>47.221299999999999</v>
+      </c>
+      <c r="F59" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="37"/>
+      <c r="H59" s="56"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="D59" s="54">
-        <v>41.256599999999999</v>
-      </c>
-      <c r="E59" s="54">
-        <v>47.221299999999999</v>
-      </c>
-      <c r="F59" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="40"/>
-      <c r="H59" s="59"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="B60" s="47" t="s">
+      <c r="C60" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C60" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60" s="55">
+      <c r="D60" s="52">
         <v>41.0672</v>
       </c>
-      <c r="E60" s="55">
+      <c r="E60" s="52">
         <v>47.792400000000001</v>
       </c>
-      <c r="F60" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="G60" s="61"/>
-      <c r="H60" s="62"/>
+      <c r="F60" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="58"/>
+      <c r="H60" s="59"/>
     </row>
     <row r="61" spans="1:8" ht="15.75">
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>